<commit_message>
Matriz de trazabilidad con estados y comentarios
</commit_message>
<xml_diff>
--- a/Material de apoyo/Grupo4_matriz_de_trazabilidad.xlsx
+++ b/Material de apoyo/Grupo4_matriz_de_trazabilidad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\INACAP\SEPTIMO SEMESTRE\TALLER DE PROYECTO DE SOFTWARE\UNIDAD 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E242C6-BA8A-4CC7-BDD8-A32E67698DD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0D0D70-543F-4134-BFDD-EB8C8A54E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41F25F60-76D7-44AC-81D5-9C172A209EC2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -250,13 +250,52 @@
   </si>
   <si>
     <t>El ID, en el caso de las cajas chicas, se conforma desde el tipo (letra G, O, OF y C correspondientemente), el número de obra u oficina (53) y, finalmente, el número de caja (-0N). Ejemplo: O553-01. Las obras reciben un ID manualmente, ya que la empresa crea su identificador, las maquinarias utilizan el identificar otorgado por la empresa, los usuarios su rut y los gastos el número de folio del comprobante.</t>
+  </si>
+  <si>
+    <t>COMENTARIO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>Está listo, falta la validación del rut y verificar validaciones</t>
+  </si>
+  <si>
+    <t>Falta la actualización de la tabla y mejorar las validaciones de los datos</t>
+  </si>
+  <si>
+    <t>Falta implementar la actualización de datos</t>
+  </si>
+  <si>
+    <t>No se ha desarrollado</t>
+  </si>
+  <si>
+    <t>Walesca Campos// cambiado a Moris</t>
+  </si>
+  <si>
+    <t>Agregar botón a cada columna</t>
+  </si>
+  <si>
+    <t>Existe pero no se ha implementado en el repositorio</t>
+  </si>
+  <si>
+    <t>Existe pero no funciona</t>
+  </si>
+  <si>
+    <t>Faltan ajustes a la validación</t>
+  </si>
+  <si>
+    <t>No se ha implementado, pero está desarrollado</t>
+  </si>
+  <si>
+    <t>Requiere de gastos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,8 +319,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,8 +346,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -349,11 +413,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -394,6 +480,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,6 +530,7 @@
   <colors>
     <mruColors>
       <color rgb="FF000099"/>
+      <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
   <extLst>
@@ -713,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20F1E8C-7DCA-45BD-B4F7-BAF7408582A3}">
-  <dimension ref="B2:H21"/>
+  <dimension ref="A2:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,10 +857,12 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -754,8 +884,14 @@
       <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -777,54 +913,67 @@
       <c r="H3" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="21"/>
+      <c r="J3" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="F4" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I4" s="31"/>
+      <c r="J4" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="28"/>
+    </row>
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I5" s="34"/>
+      <c r="J5" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -846,8 +995,10 @@
       <c r="H6" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I6" s="19"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -869,54 +1020,65 @@
       <c r="H7" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I7" s="14"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="F8" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I8" s="35"/>
+      <c r="J8" s="32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="F9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="33" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I9" s="36"/>
+      <c r="J9" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -938,31 +1100,38 @@
       <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10" s="17"/>
+      <c r="J10" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I11" s="29"/>
+      <c r="J11" s="25"/>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -982,10 +1151,14 @@
         <v>63</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1007,8 +1180,12 @@
       <c r="H13" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I13" s="16"/>
+      <c r="J13" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1030,8 +1207,10 @@
       <c r="H14" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I14" s="19"/>
+      <c r="J14" s="22"/>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1053,8 +1232,12 @@
       <c r="H15" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I15" s="15"/>
+      <c r="J15" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1076,8 +1259,10 @@
       <c r="H16" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I16" s="19"/>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1099,8 +1284,12 @@
       <c r="H17" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I17" s="14"/>
+      <c r="J17" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1120,10 +1309,14 @@
         <v>63</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1145,8 +1338,10 @@
       <c r="H19" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I19" s="16"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1168,8 +1363,10 @@
       <c r="H20" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="17"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1191,8 +1388,11 @@
       <c r="H21" s="10" t="s">
         <v>67</v>
       </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>